<commit_message>
cumulative update after revised second variation of ppe, hhs analysis
</commit_message>
<xml_diff>
--- a/data/SNS_PPE_REPORT.xlsx
+++ b/data/SNS_PPE_REPORT.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITREPOS\gh_kessler\covid_statesupplies\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITREPOS\bb_kessler\covid_statesupplies_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25A8A9-4280-4AEC-96A0-143E09FDFE29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8B0682-B11B-4947-BF7A-2065FEB13FC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="combinedstatelocal" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$56</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="88">
   <si>
     <t> California</t>
   </si>
@@ -305,7 +306,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -368,7 +369,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -406,14 +407,17 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -758,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7234,6 +7238,2064 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA47E64-33E6-4864-898D-0FD63555F4EB}">
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" style="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="14">
+        <v>4779736</v>
+      </c>
+      <c r="D2" s="14">
+        <v>2499</v>
+      </c>
+      <c r="E2" s="14">
+        <v>152412</v>
+      </c>
+      <c r="F2" s="14">
+        <v>362580</v>
+      </c>
+      <c r="G2" s="14">
+        <v>72922</v>
+      </c>
+      <c r="H2" s="14">
+        <v>59699</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1939</v>
+      </c>
+      <c r="J2" s="14">
+        <v>305359</v>
+      </c>
+      <c r="K2" s="14">
+        <v>0</v>
+      </c>
+      <c r="L2" s="14">
+        <v>0</v>
+      </c>
+      <c r="M2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="14">
+        <v>710231</v>
+      </c>
+      <c r="D3" s="14">
+        <v>226</v>
+      </c>
+      <c r="E3" s="14">
+        <v>74115</v>
+      </c>
+      <c r="F3" s="14">
+        <v>176063</v>
+      </c>
+      <c r="G3" s="14">
+        <v>37405</v>
+      </c>
+      <c r="H3" s="14">
+        <v>30742</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1791</v>
+      </c>
+      <c r="J3" s="14">
+        <v>202253</v>
+      </c>
+      <c r="K3" s="14">
+        <v>50</v>
+      </c>
+      <c r="L3" s="14">
+        <v>60</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="14">
+        <v>6392017</v>
+      </c>
+      <c r="D4" s="14">
+        <v>2726</v>
+      </c>
+      <c r="E4" s="14">
+        <v>183432</v>
+      </c>
+      <c r="F4" s="14">
+        <v>436476</v>
+      </c>
+      <c r="G4" s="14">
+        <v>86993</v>
+      </c>
+      <c r="H4" s="14">
+        <v>71172</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1998</v>
+      </c>
+      <c r="J4" s="14">
+        <v>346209</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2915918</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1071</v>
+      </c>
+      <c r="E5" s="14">
+        <v>116552</v>
+      </c>
+      <c r="F5" s="14">
+        <v>277156</v>
+      </c>
+      <c r="G5" s="14">
+        <v>56655</v>
+      </c>
+      <c r="H5" s="14">
+        <v>46437</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1871</v>
+      </c>
+      <c r="J5" s="14">
+        <v>258137</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5029196</v>
+      </c>
+      <c r="D6" s="14">
+        <v>5655</v>
+      </c>
+      <c r="E6" s="14">
+        <v>217661</v>
+      </c>
+      <c r="F6" s="14">
+        <v>517525</v>
+      </c>
+      <c r="G6" s="14">
+        <v>106305</v>
+      </c>
+      <c r="H6" s="14">
+        <v>87161</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3711</v>
+      </c>
+      <c r="J6" s="14">
+        <v>495936</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="14">
+        <v>3574097</v>
+      </c>
+      <c r="D7" s="14">
+        <v>8781</v>
+      </c>
+      <c r="E7" s="14">
+        <v>189665</v>
+      </c>
+      <c r="F7" s="14">
+        <v>450833</v>
+      </c>
+      <c r="G7" s="14">
+        <v>93606</v>
+      </c>
+      <c r="H7" s="14">
+        <v>76807</v>
+      </c>
+      <c r="I7" s="14">
+        <v>3658</v>
+      </c>
+      <c r="J7" s="14">
+        <v>459069</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14">
+        <v>50</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="14">
+        <v>897934</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1116</v>
+      </c>
+      <c r="E8" s="14">
+        <v>77434</v>
+      </c>
+      <c r="F8" s="14">
+        <v>184666</v>
+      </c>
+      <c r="G8" s="14">
+        <v>39044</v>
+      </c>
+      <c r="H8" s="14">
+        <v>32077</v>
+      </c>
+      <c r="I8" s="14">
+        <v>1765</v>
+      </c>
+      <c r="J8" s="14">
+        <v>207008</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="14">
+        <v>18801310</v>
+      </c>
+      <c r="D9" s="14">
+        <v>15234</v>
+      </c>
+      <c r="E9" s="14">
+        <v>482635</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1148742</v>
+      </c>
+      <c r="G9" s="14">
+        <v>226500</v>
+      </c>
+      <c r="H9" s="14">
+        <v>185159</v>
+      </c>
+      <c r="I9" s="14">
+        <v>4212</v>
+      </c>
+      <c r="J9" s="14">
+        <v>844872</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14">
+        <v>200</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="14">
+        <v>9687653</v>
+      </c>
+      <c r="D10" s="14">
+        <v>10446</v>
+      </c>
+      <c r="E10" s="14">
+        <v>307289</v>
+      </c>
+      <c r="F10" s="14">
+        <v>731036</v>
+      </c>
+      <c r="G10" s="14">
+        <v>146961</v>
+      </c>
+      <c r="H10" s="14">
+        <v>120309</v>
+      </c>
+      <c r="I10" s="14">
+        <v>3881</v>
+      </c>
+      <c r="J10" s="14">
+        <v>613965</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14">
+        <v>150</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1360301</v>
+      </c>
+      <c r="D11" s="14">
+        <v>377</v>
+      </c>
+      <c r="E11" s="14">
+        <v>86622</v>
+      </c>
+      <c r="F11" s="14">
+        <v>205858</v>
+      </c>
+      <c r="G11" s="14">
+        <v>43079</v>
+      </c>
+      <c r="H11" s="14">
+        <v>35367</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1815</v>
+      </c>
+      <c r="J11" s="14">
+        <v>218723</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1567582</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1232</v>
+      </c>
+      <c r="E12" s="14">
+        <v>90610</v>
+      </c>
+      <c r="F12" s="14">
+        <v>215358</v>
+      </c>
+      <c r="G12" s="14">
+        <v>44888</v>
+      </c>
+      <c r="H12" s="14">
+        <v>36842</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1822</v>
+      </c>
+      <c r="J12" s="14">
+        <v>223975</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="14">
+        <v>6483802</v>
+      </c>
+      <c r="D13" s="14">
+        <v>5943</v>
+      </c>
+      <c r="E13" s="15">
+        <v>185198</v>
+      </c>
+      <c r="F13" s="15">
+        <v>440683</v>
+      </c>
+      <c r="G13" s="15">
+        <v>87794</v>
+      </c>
+      <c r="H13" s="15">
+        <v>71825</v>
+      </c>
+      <c r="I13" s="15">
+        <v>2001</v>
+      </c>
+      <c r="J13" s="15">
+        <v>348534</v>
+      </c>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3046355</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1145</v>
+      </c>
+      <c r="E14" s="14">
+        <v>119062</v>
+      </c>
+      <c r="F14" s="14">
+        <v>283134</v>
+      </c>
+      <c r="G14" s="14">
+        <v>57794</v>
+      </c>
+      <c r="H14" s="14">
+        <v>47365</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1876</v>
+      </c>
+      <c r="J14" s="14">
+        <v>261442</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2853118</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1076</v>
+      </c>
+      <c r="E15" s="14">
+        <v>115344</v>
+      </c>
+      <c r="F15" s="14">
+        <v>274278</v>
+      </c>
+      <c r="G15" s="14">
+        <v>56107</v>
+      </c>
+      <c r="H15" s="14">
+        <v>45990</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1869</v>
+      </c>
+      <c r="J15" s="14">
+        <v>256546</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="14">
+        <v>4339367</v>
+      </c>
+      <c r="D16" s="14">
+        <v>1346</v>
+      </c>
+      <c r="E16" s="14">
+        <v>143939</v>
+      </c>
+      <c r="F16" s="14">
+        <v>342397</v>
+      </c>
+      <c r="G16" s="14">
+        <v>69078</v>
+      </c>
+      <c r="H16" s="14">
+        <v>56566</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1923</v>
+      </c>
+      <c r="J16" s="14">
+        <v>294202</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14">
+        <v>0</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="14">
+        <v>4533372</v>
+      </c>
+      <c r="D17" s="14">
+        <v>17030</v>
+      </c>
+      <c r="E17" s="14">
+        <v>208122</v>
+      </c>
+      <c r="F17" s="14">
+        <v>494800</v>
+      </c>
+      <c r="G17" s="14">
+        <v>101978</v>
+      </c>
+      <c r="H17" s="14">
+        <v>83633</v>
+      </c>
+      <c r="I17" s="14">
+        <v>3693</v>
+      </c>
+      <c r="J17" s="14">
+        <v>483373</v>
+      </c>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14">
+        <v>150</v>
+      </c>
+      <c r="M17" s="14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1328361</v>
+      </c>
+      <c r="D18" s="14">
+        <v>537</v>
+      </c>
+      <c r="E18" s="14">
+        <v>86008</v>
+      </c>
+      <c r="F18" s="14">
+        <v>204394</v>
+      </c>
+      <c r="G18" s="14">
+        <v>42800</v>
+      </c>
+      <c r="H18" s="14">
+        <v>35140</v>
+      </c>
+      <c r="I18" s="14">
+        <v>1813</v>
+      </c>
+      <c r="J18" s="14">
+        <v>217914</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="14">
+        <v>5773552</v>
+      </c>
+      <c r="D19" s="14">
+        <v>6185</v>
+      </c>
+      <c r="E19" s="14">
+        <v>171533</v>
+      </c>
+      <c r="F19" s="14">
+        <v>408130</v>
+      </c>
+      <c r="G19" s="14">
+        <v>81595</v>
+      </c>
+      <c r="H19" s="14">
+        <v>66771</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1975</v>
+      </c>
+      <c r="J19" s="14">
+        <v>330539</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14">
+        <v>120</v>
+      </c>
+      <c r="M19" s="14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="14">
+        <v>6547629</v>
+      </c>
+      <c r="D20" s="14">
+        <v>16567</v>
+      </c>
+      <c r="E20" s="14">
+        <v>246876</v>
+      </c>
+      <c r="F20" s="14">
+        <v>587120</v>
+      </c>
+      <c r="G20" s="14">
+        <v>119557</v>
+      </c>
+      <c r="H20" s="14">
+        <v>97965</v>
+      </c>
+      <c r="I20" s="14">
+        <v>3766</v>
+      </c>
+      <c r="J20" s="14">
+        <v>534408</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14">
+        <v>0</v>
+      </c>
+      <c r="M20" s="14">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="14">
+        <v>9883640</v>
+      </c>
+      <c r="D21" s="14">
+        <v>20346</v>
+      </c>
+      <c r="E21" s="14">
+        <v>311060</v>
+      </c>
+      <c r="F21" s="14">
+        <v>740018</v>
+      </c>
+      <c r="G21" s="14">
+        <v>148672</v>
+      </c>
+      <c r="H21" s="14">
+        <v>121704</v>
+      </c>
+      <c r="I21" s="14">
+        <v>3888</v>
+      </c>
+      <c r="J21" s="14">
+        <v>618930</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14">
+        <v>400</v>
+      </c>
+      <c r="M21" s="14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="14">
+        <v>5303925</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1242</v>
+      </c>
+      <c r="E22" s="14">
+        <v>162497</v>
+      </c>
+      <c r="F22" s="14">
+        <v>386606</v>
+      </c>
+      <c r="G22" s="14">
+        <v>77497</v>
+      </c>
+      <c r="H22" s="14">
+        <v>63429</v>
+      </c>
+      <c r="I22" s="14">
+        <v>1958</v>
+      </c>
+      <c r="J22" s="14">
+        <v>318641</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14">
+        <v>0</v>
+      </c>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2967297</v>
+      </c>
+      <c r="D23" s="14">
+        <v>2260</v>
+      </c>
+      <c r="E23" s="14">
+        <v>117541</v>
+      </c>
+      <c r="F23" s="14">
+        <v>279511</v>
+      </c>
+      <c r="G23" s="14">
+        <v>57104</v>
+      </c>
+      <c r="H23" s="14">
+        <v>46802</v>
+      </c>
+      <c r="I23" s="14">
+        <v>1873</v>
+      </c>
+      <c r="J23" s="14">
+        <v>259439</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14">
+        <v>0</v>
+      </c>
+      <c r="M23" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="14">
+        <v>5988927</v>
+      </c>
+      <c r="D24" s="14">
+        <v>3327</v>
+      </c>
+      <c r="E24" s="14">
+        <v>175676</v>
+      </c>
+      <c r="F24" s="14">
+        <v>418001</v>
+      </c>
+      <c r="G24" s="14">
+        <v>83475</v>
+      </c>
+      <c r="H24" s="14">
+        <v>68303</v>
+      </c>
+      <c r="I24" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J24" s="14">
+        <v>335996</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14">
+        <v>0</v>
+      </c>
+      <c r="M24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="14">
+        <v>989415</v>
+      </c>
+      <c r="D25" s="14">
+        <v>352</v>
+      </c>
+      <c r="E25" s="14">
+        <v>79486</v>
+      </c>
+      <c r="F25" s="14">
+        <v>188859</v>
+      </c>
+      <c r="G25" s="14">
+        <v>39842</v>
+      </c>
+      <c r="H25" s="14">
+        <v>32728</v>
+      </c>
+      <c r="I25" s="14">
+        <v>1801</v>
+      </c>
+      <c r="J25" s="14">
+        <v>209326</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14">
+        <v>0</v>
+      </c>
+      <c r="M25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1826341</v>
+      </c>
+      <c r="D26" s="14">
+        <v>523</v>
+      </c>
+      <c r="E26" s="14">
+        <v>95589</v>
+      </c>
+      <c r="F26" s="14">
+        <v>227218</v>
+      </c>
+      <c r="G26" s="14">
+        <v>47146</v>
+      </c>
+      <c r="H26" s="14">
+        <v>38684</v>
+      </c>
+      <c r="I26" s="14">
+        <v>1831</v>
+      </c>
+      <c r="J26" s="14">
+        <v>230531</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14">
+        <v>0</v>
+      </c>
+      <c r="M26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="14">
+        <v>2700551</v>
+      </c>
+      <c r="D27" s="14">
+        <v>2318</v>
+      </c>
+      <c r="E27" s="14">
+        <v>112408</v>
+      </c>
+      <c r="F27" s="14">
+        <v>267285</v>
+      </c>
+      <c r="G27" s="14">
+        <v>54776</v>
+      </c>
+      <c r="H27" s="14">
+        <v>44904</v>
+      </c>
+      <c r="I27" s="14">
+        <v>1863</v>
+      </c>
+      <c r="J27" s="14">
+        <v>252680</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14">
+        <v>0</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1316470</v>
+      </c>
+      <c r="D28" s="14">
+        <v>788</v>
+      </c>
+      <c r="E28" s="14">
+        <v>85779</v>
+      </c>
+      <c r="F28" s="14">
+        <v>203849</v>
+      </c>
+      <c r="G28" s="14">
+        <v>42696</v>
+      </c>
+      <c r="H28" s="14">
+        <v>35056</v>
+      </c>
+      <c r="I28" s="14">
+        <v>1813</v>
+      </c>
+      <c r="J28" s="14">
+        <v>217613</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14">
+        <v>0</v>
+      </c>
+      <c r="M28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="14">
+        <v>8791894</v>
+      </c>
+      <c r="D29" s="14">
+        <v>47437</v>
+      </c>
+      <c r="E29" s="14">
+        <v>290055</v>
+      </c>
+      <c r="F29" s="14">
+        <v>689981</v>
+      </c>
+      <c r="G29" s="14">
+        <v>139144</v>
+      </c>
+      <c r="H29" s="14">
+        <v>113935</v>
+      </c>
+      <c r="I29" s="14">
+        <v>3848</v>
+      </c>
+      <c r="J29" s="14">
+        <v>591269</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14">
+        <v>1100</v>
+      </c>
+      <c r="M29" s="14">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="14">
+        <v>2059179</v>
+      </c>
+      <c r="D30" s="14">
+        <v>865</v>
+      </c>
+      <c r="E30" s="14">
+        <v>100068</v>
+      </c>
+      <c r="F30" s="14">
+        <v>237889</v>
+      </c>
+      <c r="G30" s="14">
+        <v>49178</v>
+      </c>
+      <c r="H30" s="14">
+        <v>40340</v>
+      </c>
+      <c r="I30" s="14">
+        <v>1840</v>
+      </c>
+      <c r="J30" s="14">
+        <v>236430</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14">
+        <v>0</v>
+      </c>
+      <c r="M30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="14">
+        <v>9535483</v>
+      </c>
+      <c r="D31" s="14">
+        <v>3651</v>
+      </c>
+      <c r="E31" s="14">
+        <v>243912</v>
+      </c>
+      <c r="F31" s="14">
+        <v>580550</v>
+      </c>
+      <c r="G31" s="14">
+        <v>114427</v>
+      </c>
+      <c r="H31" s="14">
+        <v>93540</v>
+      </c>
+      <c r="I31" s="14">
+        <v>2112</v>
+      </c>
+      <c r="J31" s="14">
+        <v>425853</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14">
+        <v>0</v>
+      </c>
+      <c r="M31" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="14">
+        <v>672591</v>
+      </c>
+      <c r="D32" s="14">
+        <v>251</v>
+      </c>
+      <c r="E32" s="14">
+        <v>73391</v>
+      </c>
+      <c r="F32" s="14">
+        <v>174338</v>
+      </c>
+      <c r="G32" s="14">
+        <v>37077</v>
+      </c>
+      <c r="H32" s="14">
+        <v>30474</v>
+      </c>
+      <c r="I32" s="14">
+        <v>1789</v>
+      </c>
+      <c r="J32" s="14">
+        <v>201299</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14">
+        <v>0</v>
+      </c>
+      <c r="M32" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="14">
+        <v>11536504</v>
+      </c>
+      <c r="D33" s="14">
+        <v>5148</v>
+      </c>
+      <c r="E33" s="14">
+        <v>282411</v>
+      </c>
+      <c r="F33" s="14">
+        <v>672263</v>
+      </c>
+      <c r="G33" s="14">
+        <v>131891</v>
+      </c>
+      <c r="H33" s="14">
+        <v>107778</v>
+      </c>
+      <c r="I33" s="14">
+        <v>2185</v>
+      </c>
+      <c r="J33" s="14">
+        <v>476552</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14">
+        <v>0</v>
+      </c>
+      <c r="M33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="14">
+        <v>3751351</v>
+      </c>
+      <c r="D34" s="14">
+        <v>1524</v>
+      </c>
+      <c r="E34" s="14">
+        <v>132626</v>
+      </c>
+      <c r="F34" s="14">
+        <v>315447</v>
+      </c>
+      <c r="G34" s="14">
+        <v>63947</v>
+      </c>
+      <c r="H34" s="14">
+        <v>52381</v>
+      </c>
+      <c r="I34" s="14">
+        <v>1902</v>
+      </c>
+      <c r="J34" s="14">
+        <v>279304</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14">
+        <v>0</v>
+      </c>
+      <c r="M34" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="14">
+        <v>3831074</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1239</v>
+      </c>
+      <c r="E35" s="14">
+        <v>134159</v>
+      </c>
+      <c r="F35" s="14">
+        <v>319100</v>
+      </c>
+      <c r="G35" s="14">
+        <v>64642</v>
+      </c>
+      <c r="H35" s="14">
+        <v>52949</v>
+      </c>
+      <c r="I35" s="14">
+        <v>1904</v>
+      </c>
+      <c r="J35" s="14">
+        <v>281324</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14">
+        <v>140</v>
+      </c>
+      <c r="M35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="14">
+        <v>12702379</v>
+      </c>
+      <c r="D36" s="14">
+        <v>16239</v>
+      </c>
+      <c r="E36" s="14">
+        <v>365293</v>
+      </c>
+      <c r="F36" s="14">
+        <v>869210</v>
+      </c>
+      <c r="G36" s="14">
+        <v>173272</v>
+      </c>
+      <c r="H36" s="14">
+        <v>141761</v>
+      </c>
+      <c r="I36" s="14">
+        <v>3990</v>
+      </c>
+      <c r="J36" s="14">
+        <v>690347</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14">
+        <v>0</v>
+      </c>
+      <c r="M36" s="14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1052567</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1450</v>
+      </c>
+      <c r="E37" s="14">
+        <v>213486</v>
+      </c>
+      <c r="F37" s="14">
+        <v>338003</v>
+      </c>
+      <c r="G37" s="14">
+        <v>65393</v>
+      </c>
+      <c r="H37" s="14">
+        <v>58178</v>
+      </c>
+      <c r="I37" s="14">
+        <v>1803</v>
+      </c>
+      <c r="J37" s="14">
+        <v>335926</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14">
+        <v>0</v>
+      </c>
+      <c r="M37" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="14">
+        <v>4625364</v>
+      </c>
+      <c r="D38" s="14">
+        <v>2552</v>
+      </c>
+      <c r="E38" s="14">
+        <v>149442</v>
+      </c>
+      <c r="F38" s="14">
+        <v>355505</v>
+      </c>
+      <c r="G38" s="14">
+        <v>71574</v>
+      </c>
+      <c r="H38" s="14">
+        <v>58601</v>
+      </c>
+      <c r="I38" s="14">
+        <v>1933</v>
+      </c>
+      <c r="J38" s="14">
+        <v>301448</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14">
+        <v>0</v>
+      </c>
+      <c r="M38" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="14">
+        <v>814180</v>
+      </c>
+      <c r="D39" s="14">
+        <v>393</v>
+      </c>
+      <c r="E39" s="14">
+        <v>76115</v>
+      </c>
+      <c r="F39" s="14">
+        <v>180827</v>
+      </c>
+      <c r="G39" s="14">
+        <v>38313</v>
+      </c>
+      <c r="H39" s="14">
+        <v>31481</v>
+      </c>
+      <c r="I39" s="14">
+        <v>1795</v>
+      </c>
+      <c r="J39" s="14">
+        <v>204886</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14">
+        <v>0</v>
+      </c>
+      <c r="M39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="14">
+        <v>6346105</v>
+      </c>
+      <c r="D40" s="14">
+        <v>4362</v>
+      </c>
+      <c r="E40" s="14">
+        <v>242998</v>
+      </c>
+      <c r="F40" s="14">
+        <v>577883</v>
+      </c>
+      <c r="G40" s="14">
+        <v>117798</v>
+      </c>
+      <c r="H40" s="14">
+        <v>96532</v>
+      </c>
+      <c r="I40" s="14">
+        <v>3759</v>
+      </c>
+      <c r="J40" s="14">
+        <v>529302</v>
+      </c>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14">
+        <v>0</v>
+      </c>
+      <c r="M40" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="14">
+        <v>25145561</v>
+      </c>
+      <c r="D41" s="14">
+        <v>9353</v>
+      </c>
+      <c r="E41" s="14">
+        <v>604698</v>
+      </c>
+      <c r="F41" s="14">
+        <v>1439517</v>
+      </c>
+      <c r="G41" s="14">
+        <v>281869</v>
+      </c>
+      <c r="H41" s="14">
+        <v>230303</v>
+      </c>
+      <c r="I41" s="14">
+        <v>4443</v>
+      </c>
+      <c r="J41" s="14">
+        <v>1005613</v>
+      </c>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14">
+        <v>0</v>
+      </c>
+      <c r="M41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="14">
+        <v>2763885</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1916</v>
+      </c>
+      <c r="E42" s="14">
+        <v>113627</v>
+      </c>
+      <c r="F42" s="14">
+        <v>270188</v>
+      </c>
+      <c r="G42" s="14">
+        <v>55329</v>
+      </c>
+      <c r="H42" s="14">
+        <v>45355</v>
+      </c>
+      <c r="I42" s="14">
+        <v>1866</v>
+      </c>
+      <c r="J42" s="14">
+        <v>254285</v>
+      </c>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14">
+        <v>0</v>
+      </c>
+      <c r="M42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="14">
+        <v>625741</v>
+      </c>
+      <c r="D43" s="14">
+        <v>605</v>
+      </c>
+      <c r="E43" s="14">
+        <v>132939</v>
+      </c>
+      <c r="F43" s="14">
+        <v>315702</v>
+      </c>
+      <c r="G43" s="14">
+        <v>67874</v>
+      </c>
+      <c r="H43" s="14">
+        <v>55828</v>
+      </c>
+      <c r="I43" s="14">
+        <v>3551</v>
+      </c>
+      <c r="J43" s="14">
+        <v>384368</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14">
+        <v>0</v>
+      </c>
+      <c r="M43" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="14">
+        <v>8001024</v>
+      </c>
+      <c r="D44" s="14">
+        <v>4042</v>
+      </c>
+      <c r="E44" s="14">
+        <v>214389</v>
+      </c>
+      <c r="F44" s="14">
+        <v>510222</v>
+      </c>
+      <c r="G44" s="14">
+        <v>101035</v>
+      </c>
+      <c r="H44" s="14">
+        <v>82621</v>
+      </c>
+      <c r="I44" s="14">
+        <v>2056</v>
+      </c>
+      <c r="J44" s="14">
+        <v>386975</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14">
+        <v>0</v>
+      </c>
+      <c r="M44" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="14">
+        <v>6724540</v>
+      </c>
+      <c r="D45" s="14">
+        <v>9097</v>
+      </c>
+      <c r="E45" s="14">
+        <v>489959</v>
+      </c>
+      <c r="F45" s="14">
+        <v>794428</v>
+      </c>
+      <c r="G45" s="14">
+        <v>126201</v>
+      </c>
+      <c r="H45" s="14">
+        <v>159225</v>
+      </c>
+      <c r="I45" s="14">
+        <v>3773</v>
+      </c>
+      <c r="J45" s="14">
+        <v>608890</v>
+      </c>
+      <c r="K45" s="14">
+        <v>50</v>
+      </c>
+      <c r="L45" s="14">
+        <v>500</v>
+      </c>
+      <c r="M45" s="14">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="14">
+        <v>1852994</v>
+      </c>
+      <c r="D46" s="14">
+        <v>412</v>
+      </c>
+      <c r="E46" s="14">
+        <v>96101</v>
+      </c>
+      <c r="F46" s="14">
+        <v>228439</v>
+      </c>
+      <c r="G46" s="14">
+        <v>47379</v>
+      </c>
+      <c r="H46" s="14">
+        <v>38873</v>
+      </c>
+      <c r="I46" s="14">
+        <v>1832</v>
+      </c>
+      <c r="J46" s="14">
+        <v>231206</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14">
+        <v>0</v>
+      </c>
+      <c r="M46" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="14">
+        <v>5686986</v>
+      </c>
+      <c r="D47" s="14">
+        <v>2756</v>
+      </c>
+      <c r="E47" s="14">
+        <v>169867</v>
+      </c>
+      <c r="F47" s="14">
+        <v>404162</v>
+      </c>
+      <c r="G47" s="14">
+        <v>80840</v>
+      </c>
+      <c r="H47" s="14">
+        <v>66155</v>
+      </c>
+      <c r="I47" s="14">
+        <v>1972</v>
+      </c>
+      <c r="J47" s="14">
+        <v>328346</v>
+      </c>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14">
+        <v>0</v>
+      </c>
+      <c r="M47" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="14">
+        <v>563626</v>
+      </c>
+      <c r="D48" s="14">
+        <v>230</v>
+      </c>
+      <c r="E48" s="14">
+        <v>71294</v>
+      </c>
+      <c r="F48" s="14">
+        <v>169344</v>
+      </c>
+      <c r="G48" s="14">
+        <v>36126</v>
+      </c>
+      <c r="H48" s="14">
+        <v>29699</v>
+      </c>
+      <c r="I48" s="14">
+        <v>1786</v>
+      </c>
+      <c r="J48" s="14">
+        <v>198538</v>
+      </c>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14">
+        <v>0</v>
+      </c>
+      <c r="M48" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="14">
+        <v>601723</v>
+      </c>
+      <c r="D49" s="14">
+        <v>1440</v>
+      </c>
+      <c r="E49" s="14">
+        <v>132477</v>
+      </c>
+      <c r="F49" s="14">
+        <v>314601</v>
+      </c>
+      <c r="G49" s="14">
+        <v>67664</v>
+      </c>
+      <c r="H49" s="14">
+        <v>55657</v>
+      </c>
+      <c r="I49" s="14">
+        <v>3550</v>
+      </c>
+      <c r="J49" s="14">
+        <v>383760</v>
+      </c>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14">
+        <v>0</v>
+      </c>
+      <c r="M49" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="17">
+        <v>47072561</v>
+      </c>
+      <c r="D50" s="17">
+        <v>24487</v>
+      </c>
+      <c r="E50" s="17">
+        <v>1087021</v>
+      </c>
+      <c r="F50" s="17">
+        <v>2588008</v>
+      </c>
+      <c r="G50" s="17">
+        <v>504442</v>
+      </c>
+      <c r="H50" s="17">
+        <v>412017</v>
+      </c>
+      <c r="I50" s="17">
+        <v>7006</v>
+      </c>
+      <c r="J50" s="17">
+        <v>1745422</v>
+      </c>
+      <c r="K50"/>
+      <c r="L50" s="17">
+        <v>170</v>
+      </c>
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="17">
+        <v>15526230</v>
+      </c>
+      <c r="D51" s="17">
+        <v>21177</v>
+      </c>
+      <c r="E51" s="17">
+        <v>540523</v>
+      </c>
+      <c r="F51" s="17">
+        <v>1285657</v>
+      </c>
+      <c r="G51" s="17">
+        <v>260330</v>
+      </c>
+      <c r="H51" s="17">
+        <v>213230</v>
+      </c>
+      <c r="I51" s="17">
+        <v>7621</v>
+      </c>
+      <c r="J51" s="17">
+        <v>1130407</v>
+      </c>
+      <c r="K51"/>
+      <c r="L51" s="17">
+        <v>450</v>
+      </c>
+      <c r="M51"/>
+    </row>
+    <row r="52" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="17">
+        <v>27553235</v>
+      </c>
+      <c r="D52" s="17">
+        <v>229520</v>
+      </c>
+      <c r="E52" s="17">
+        <v>1096922</v>
+      </c>
+      <c r="F52" s="17">
+        <v>1836891</v>
+      </c>
+      <c r="G52" s="17">
+        <v>365295</v>
+      </c>
+      <c r="H52" s="17">
+        <v>298811</v>
+      </c>
+      <c r="I52" s="17">
+        <v>8059</v>
+      </c>
+      <c r="J52" s="17">
+        <v>1435129</v>
+      </c>
+      <c r="K52"/>
+      <c r="L52" s="17">
+        <v>4400</v>
+      </c>
+      <c r="M52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7416,18 +9478,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7449,6 +9511,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3F0FAA-35E9-455A-9815-B46ED4241644}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D5AB72-FF8D-43E0-A8B8-3E744206C489}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="08807ec3-19ab-45f8-86fd-9385dec94cf5"/>
@@ -7462,12 +9532,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3F0FAA-35E9-455A-9815-B46ED4241644}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>